<commit_message>
Update and Upload Product Tasks
</commit_message>
<xml_diff>
--- a/lib/jewellery.xlsx
+++ b/lib/jewellery.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Brand</t>
   </si>
@@ -100,19 +100,16 @@
     <t xml:space="preserve">Yoko London</t>
   </si>
   <si>
-    <t xml:space="preserve">DUET001-627-FGY</t>
+    <t xml:space="preserve">Q2091NLET-7F</t>
   </si>
   <si>
-    <t xml:space="preserve">Novus</t>
+    <t xml:space="preserve">Trend</t>
   </si>
   <si>
-    <t xml:space="preserve">Duet South Sea Pearl Earrings</t>
+    <t xml:space="preserve">Freshwater Pearl and Diamond Necklace</t>
   </si>
   <si>
-    <t xml:space="preserve">Each piece in our Novus collection is bold and unique. Our striking Duet pearl earrings offer a contemporary way to wear pearls. The larger South Sea pearl sits behind the lobe, whereas the smaller pearl sits proudly at the front of the ear. These pearl earrings can be styled casually to achieve an effortless glamour, or they can be worn to add modern elegance to your favourite evening look.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call For Price</t>
+    <t xml:space="preserve">Putting style at the forefront of each design, our Trend collection is perfect for the modern woman. This 18ct white gold necklace features high quality 4-6.5mm Freshwater pearls, accentuated by scintillating diamonds. A modern 'Y'-shaped silhouette is both elegant and contemporary, and will elevate any outfit. </t>
   </si>
   <si>
     <t xml:space="preserve">For Her</t>
@@ -121,25 +118,34 @@
     <t xml:space="preserve">Fashion Jewellery</t>
   </si>
   <si>
-    <t xml:space="preserve">Earrings</t>
+    <t xml:space="preserve">Necklace</t>
   </si>
   <si>
     <t xml:space="preserve">White Gold</t>
   </si>
   <si>
-    <t xml:space="preserve">Pearl</t>
+    <t xml:space="preserve">Pearl - Diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">Australian South Sea</t>
+    <t xml:space="preserve">0.188ct</t>
   </si>
   <si>
-    <t xml:space="preserve">9.5 - 10 x 13 - 14 mm</t>
+    <t xml:space="preserve">18K Yellow Gold</t>
   </si>
   <si>
-    <t xml:space="preserve">DUET001-627_1000.png</t>
+    <t xml:space="preserve">Freshwater</t>
   </si>
   <si>
-    <t xml:space="preserve">DUET001-627 (2)_1000.png</t>
+    <t xml:space="preserve">4 - 6.5 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2091NLET-7F_1000.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2091NLET-7F CLASP_1000.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2091NLET-7f M_1000.png</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,7 +293,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,12 +335,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,51 +449,61 @@
       <c r="A2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3" t="n">
+        <v>1560</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="P2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="T2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="U2" s="15" t="s">
         <v>37</v>
       </c>
+      <c r="V2" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="W2" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Completed all 5 task
</commit_message>
<xml_diff>
--- a/lib/jewellery.xlsx
+++ b/lib/jewellery.xlsx
@@ -654,7 +654,7 @@
     <sheetView showFormulas="false" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="false" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="X1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+      <selection pane="bottomLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -787,78 +787,80 @@
         <v>product_id</v>
       </c>
       <c r="Z1" s="9" t="str">
+        <v>inventory_item_id</v>
+      </c>
+      <c r="AA1" s="9" t="str">
         <v>metafield_Brand_id</v>
       </c>
-      <c r="AA1" s="9" t="str">
+      <c r="AB1" s="9" t="str">
         <v>metafield_Reference_Number_id</v>
       </c>
-      <c r="AB1" s="9" t="str">
+      <c r="AC1" s="9" t="str">
         <v>metafield_Collection_id</v>
       </c>
-      <c r="AC1" s="9" t="str">
+      <c r="AD1" s="9" t="str">
         <v>metafield_Product_Name_id</v>
       </c>
-      <c r="AD1" s="9" t="str">
+      <c r="AE1" s="9" t="str">
         <v>metafield_Description_id</v>
       </c>
-      <c r="AE1" s="9" t="str">
+      <c r="AF1" s="9" t="str">
         <v>metafield_Price_id</v>
       </c>
-      <c r="AF1" s="9" t="str">
+      <c r="AG1" s="9" t="str">
         <v>metafield_Price_Note_id</v>
       </c>
-      <c r="AG1" s="9" t="str">
+      <c r="AH1" s="9" t="str">
         <v>metafield_Quantity_id</v>
       </c>
-      <c r="AH1" s="9" t="str">
+      <c r="AI1" s="9" t="str">
         <v>metafield_Gender_id</v>
       </c>
-      <c r="AI1" s="9" t="str">
+      <c r="AJ1" s="9" t="str">
         <v>metafield_Function_id</v>
       </c>
-      <c r="AJ1" s="9" t="str">
+      <c r="AK1" s="9" t="str">
         <v>metafield_Category_id</v>
       </c>
-      <c r="AK1" s="9" t="str">
+      <c r="AL1" s="9" t="str">
         <v>metafield_Sub_Category_id</v>
       </c>
-      <c r="AL1" s="9" t="str">
+      <c r="AM1" s="9" t="str">
         <v>metafield_Metal_id</v>
       </c>
-      <c r="AM1" s="9" t="str">
+      <c r="AN1" s="9" t="str">
         <v>metafield_Stone_id</v>
       </c>
-      <c r="AN1" s="9" t="str">
+      <c r="AO1" s="9" t="str">
         <v>metafield_Diamond_Clarity_id</v>
       </c>
-      <c r="AO1" s="9" t="str">
+      <c r="AP1" s="9" t="str">
         <v>metafield_Total_Diamond_Weight_id</v>
       </c>
-      <c r="AP1" s="9" t="str">
+      <c r="AQ1" s="9" t="str">
         <v>metafield_Also_Available_In_id</v>
       </c>
-      <c r="AQ1" s="9" t="str">
+      <c r="AR1" s="9" t="str">
         <v>metafield_Width_id</v>
       </c>
-      <c r="AR1" s="9" t="str">
+      <c r="AS1" s="9" t="str">
         <v>metafield_Head_Size_id</v>
       </c>
-      <c r="AS1" s="9" t="str">
+      <c r="AT1" s="9" t="str">
         <v>metafield_Pearl_Type_id</v>
       </c>
-      <c r="AT1" s="9" t="str">
+      <c r="AU1" s="9" t="str">
         <v>metafield_Pearl_Size_id</v>
       </c>
-      <c r="AU1" s="9" t="str">
+      <c r="AV1" s="9" t="str">
         <v>metafield_Picture_1_id</v>
       </c>
-      <c r="AV1" s="9" t="str">
+      <c r="AW1" s="9" t="str">
         <v>metafield_Picture_2_id</v>
       </c>
-      <c r="AW1" s="9" t="str">
+      <c r="AX1" s="9" t="str">
         <v>metafield_Picture_3_id</v>
       </c>
-      <c r="AX1" s="0"/>
     </row>
     <row r="2" spans="1:50" s="10" customFormat="1" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
@@ -920,81 +922,83 @@
         <v>40</v>
       </c>
       <c r="Y2" s="10" t="str">
-        <v>7491717922985</v>
+        <v>7492350705833</v>
       </c>
       <c r="Z2" s="10" t="str">
-        <v>20897229897897</v>
+        <v>44332328911017</v>
       </c>
       <c r="AA2" s="10" t="str">
-        <v>20897229930665</v>
+        <v>20897912357033</v>
       </c>
       <c r="AB2" s="10" t="str">
-        <v>20897229963433</v>
+        <v>20897912389801</v>
       </c>
       <c r="AC2" s="10" t="str">
-        <v>20897229996201</v>
+        <v>20897912422569</v>
       </c>
       <c r="AD2" s="10" t="str">
-        <v>20897230028969</v>
+        <v>20897912455337</v>
       </c>
       <c r="AE2" s="10" t="str">
-        <v>20897230061737</v>
+        <v>20897912488105</v>
       </c>
       <c r="AF2" s="10" t="str">
-        <v>20897230094505</v>
+        <v>20897912520873</v>
       </c>
       <c r="AG2" s="10" t="str">
-        <v>20897230127273</v>
+        <v>20897912553641</v>
       </c>
       <c r="AH2" s="10" t="str">
-        <v>20897230160041</v>
+        <v>20897912586409</v>
       </c>
       <c r="AI2" s="10" t="str">
-        <v>20897230192809</v>
+        <v>20897912619177</v>
       </c>
       <c r="AJ2" s="10" t="str">
-        <v>20897230225577</v>
+        <v>20897912651945</v>
       </c>
       <c r="AK2" s="10" t="str">
-        <v>20897230258345</v>
+        <v>20897912684713</v>
       </c>
       <c r="AL2" s="10" t="str">
-        <v>20897230520489</v>
+        <v>20897912717481</v>
       </c>
       <c r="AM2" s="10" t="str">
-        <v>20897230553257</v>
+        <v>20897912783017</v>
       </c>
       <c r="AN2" s="10" t="str">
-        <v>20897230586025</v>
+        <v>20897912815785</v>
       </c>
       <c r="AO2" s="10" t="str">
-        <v>20897230618793</v>
+        <v>20897912848553</v>
       </c>
       <c r="AP2" s="10" t="str">
-        <v>20897230651561</v>
+        <v>20897912881321</v>
       </c>
       <c r="AQ2" s="10" t="str">
-        <v>20897230684329</v>
+        <v>20897912914089</v>
       </c>
       <c r="AR2" s="10" t="str">
-        <v>20897230717097</v>
+        <v>20897912946857</v>
       </c>
       <c r="AS2" s="10" t="str">
-        <v>20897230749865</v>
+        <v>20897912979625</v>
       </c>
       <c r="AT2" s="10" t="str">
-        <v>20897230848169</v>
+        <v>20897913012393</v>
       </c>
       <c r="AU2" s="10" t="str">
-        <v>20897230880937</v>
+        <v>20897913045161</v>
       </c>
       <c r="AV2" s="10" t="str">
-        <v>20897230913705</v>
+        <v>20897913077929</v>
       </c>
       <c r="AW2" s="10" t="str">
-        <v>20897230946473</v>
-      </c>
-      <c r="AX2" s="0"/>
+        <v>20897913110697</v>
+      </c>
+      <c r="AX2" s="10" t="str">
+        <v>20897913143465</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:X4635">

</xml_diff>